<commit_message>
Pedoe pick 3 linked list problem
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="2300" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>#</t>
   </si>
@@ -69,6 +69,24 @@
   </si>
   <si>
     <t>Ongoing</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>Pedoe</t>
+  </si>
+  <si>
+    <t>Reverse a single linked list</t>
+  </si>
+  <si>
+    <t>Linked List Cycle</t>
+  </si>
+  <si>
+    <t>Solve it without using extra space</t>
+  </si>
+  <si>
+    <t>Merge Two Sort Lists</t>
   </si>
 </sst>
 </file>
@@ -415,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,6 +497,72 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>206</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aton picked 3 linked list problems
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="42760" yWindow="2800" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Easy" sheetId="1" r:id="rId1"/>
+    <sheet name="Medium" sheetId="2" r:id="rId2"/>
+    <sheet name="Hard" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
   <si>
     <t>#</t>
   </si>
@@ -59,9 +61,6 @@
     <t>Aton</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Easy</t>
   </si>
   <si>
@@ -87,6 +86,18 @@
   </si>
   <si>
     <t>Merge Two Sort Lists</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Delete Node in a Linked List</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted List</t>
   </si>
 </sst>
 </file>
@@ -112,7 +123,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF00B050"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,7 +131,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="5"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -155,6 +166,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -433,20 +446,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="38.33203125" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="7" max="7" width="43.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="8" max="8" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,105 +477,293 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>234</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>206</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>206</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>141</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
+        <v>234</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>237</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="8" max="8" width="49.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="8" max="8" width="49.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
I-No picked 2 Linked list problems
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/Leetcode/Leetcode_github/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD15972-ECC0-084F-B99A-A59DA5F77810}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42760" yWindow="2800" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="21500" yWindow="6320" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
     <sheet name="Medium" sheetId="2" r:id="rId2"/>
     <sheet name="Hard" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
   <si>
     <t>#</t>
   </si>
@@ -61,9 +62,6 @@
     <t>Aton</t>
   </si>
   <si>
-    <t>Easy</t>
-  </si>
-  <si>
     <t>O(n) time complexity, O(1) space complexity</t>
   </si>
   <si>
@@ -98,13 +96,28 @@
   </si>
   <si>
     <t>Remove Duplicates from Sorted List</t>
+  </si>
+  <si>
+    <t>Intersection fo Two Linked Lists</t>
+  </si>
+  <si>
+    <t>I-No</t>
+  </si>
+  <si>
+    <t>Discussed</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Remove Linked List Elements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,6 +149,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -169,6 +190,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,6 +200,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -445,11 +470,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,10 +502,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -491,28 +516,25 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="4"/>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -520,14 +542,11 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
+      <c r="E3" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -535,23 +554,20 @@
         <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -559,23 +575,20 @@
         <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="H5" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -591,17 +604,14 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
+      <c r="E6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
         <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -609,7 +619,7 @@
         <v>237</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -617,23 +627,61 @@
       <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>12</v>
+      <c r="E7" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>160</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>203</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -665,7 +713,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -702,7 +750,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -734,7 +782,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Update INo's stack & queue assignments
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/Leetcode/Leetcode_github/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3F9A3F-2E64-8C43-8137-DD97452A8AAF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF0B7F7-C3FD-C84D-800D-02F8D67B61F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21500" yWindow="6320" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11840" yWindow="6760" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
   <si>
     <t>#</t>
   </si>
@@ -65,9 +65,6 @@
     <t>O(n) time complexity, O(1) space complexity</t>
   </si>
   <si>
-    <t>Ongoing</t>
-  </si>
-  <si>
     <t>Reverse Linked List</t>
   </si>
   <si>
@@ -117,6 +114,24 @@
   </si>
   <si>
     <t>O(n) in time and O(1) in space. Interesting.</t>
+  </si>
+  <si>
+    <t>Min Stack</t>
+  </si>
+  <si>
+    <t>On-going</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Baseball Game</t>
+  </si>
+  <si>
+    <t>Stack &amp; Queue</t>
+  </si>
+  <si>
+    <t>Task Scheduler</t>
   </si>
 </sst>
 </file>
@@ -164,12 +179,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -184,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,6 +218,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,10 +531,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -522,25 +545,28 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="F2" s="4"/>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -549,10 +575,13 @@
         <v>9</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -560,20 +589,23 @@
         <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="F4" s="4"/>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -581,20 +613,23 @@
         <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="H5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -611,10 +646,13 @@
         <v>9</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
@@ -625,7 +663,7 @@
         <v>237</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -634,10 +672,13 @@
         <v>9</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -645,22 +686,25 @@
         <v>160</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -668,22 +712,95 @@
         <v>203</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>155</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>682</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>621</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -725,7 +842,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -794,7 +911,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Pedoe picked 3 questions
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/Leetcode/Leetcode_github/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF0B7F7-C3FD-C84D-800D-02F8D67B61F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11840" yWindow="6760" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11480" yWindow="1780" windowWidth="14400" windowHeight="9660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
     <sheet name="Medium" sheetId="2" r:id="rId2"/>
     <sheet name="Hard" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="38">
   <si>
     <t>#</t>
   </si>
@@ -132,12 +131,24 @@
   </si>
   <si>
     <t>Task Scheduler</t>
+  </si>
+  <si>
+    <t>Javascript</t>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Next Greater Element II</t>
+  </si>
+  <si>
+    <t>Decoding String</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -499,11 +510,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,7 +567,9 @@
       <c r="E2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="G2" t="s">
         <v>30</v>
       </c>
@@ -600,7 +613,9 @@
       <c r="E4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="G4" t="s">
         <v>30</v>
       </c>
@@ -624,7 +639,9 @@
       <c r="E5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="G5" t="s">
         <v>30</v>
       </c>
@@ -803,6 +820,66 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>503</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>394</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -810,7 +887,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -879,7 +956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">

</xml_diff>

<commit_message>
Update INo's assignment(155 to 225)
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/Leetcode/Leetcode_github/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF0B7F7-C3FD-C84D-800D-02F8D67B61F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABD01E5-7961-C843-8428-75AB9E622FEE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11840" yWindow="6760" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>O(n) in time and O(1) in space. Interesting.</t>
   </si>
   <si>
-    <t>Min Stack</t>
-  </si>
-  <si>
     <t>On-going</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>Task Scheduler</t>
+  </si>
+  <si>
+    <t>Implement Stack using Queues</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -581,7 +581,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -602,7 +602,7 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -626,7 +626,7 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
@@ -652,7 +652,7 @@
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
@@ -678,7 +678,7 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -701,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" t="s">
         <v>27</v>
@@ -727,7 +727,7 @@
         <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
@@ -745,19 +745,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>155</v>
+        <v>225</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -768,16 +768,16 @@
         <v>682</v>
       </c>
       <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>18</v>
@@ -788,16 +788,16 @@
         <v>621</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
resubmit Pedoe 3 questions
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/Leetcode/Leetcode_github/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABD01E5-7961-C843-8428-75AB9E622FEE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11840" yWindow="6760" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
     <sheet name="Medium" sheetId="2" r:id="rId2"/>
     <sheet name="Hard" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
   <si>
     <t>#</t>
   </si>
@@ -132,13 +131,25 @@
   </si>
   <si>
     <t>Implement Stack using Queues</t>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Javascript</t>
+  </si>
+  <si>
+    <t>Next Greater Element II</t>
+  </si>
+  <si>
+    <t>Decoding String</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +189,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFED7D31"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF4472C4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -205,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -220,6 +254,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,11 +536,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,6 +840,66 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>20</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>503</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>394</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -810,7 +907,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -879,7 +976,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">

</xml_diff>

<commit_message>
Aton picked 3 stack & queue questions
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Documents/Career @US/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="13680" yWindow="460" windowWidth="23860" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="43">
   <si>
     <t>#</t>
   </si>
@@ -143,6 +143,21 @@
   </si>
   <si>
     <t>Decoding String</t>
+  </si>
+  <si>
+    <t>March 18, 2018</t>
+  </si>
+  <si>
+    <t>Implement Queue using Stacks</t>
+  </si>
+  <si>
+    <t>Next Greater Element I</t>
+  </si>
+  <si>
+    <t>Min Stack</t>
+  </si>
+  <si>
+    <t>March 25, 2018</t>
   </si>
 </sst>
 </file>
@@ -222,7 +237,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,11 +267,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -771,14 +787,16 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="A10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -841,66 +859,142 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
+      <c r="A14" s="8">
         <v>20</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
+      <c r="A15" s="8">
         <v>503</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="10">
+      <c r="A16" s="8">
         <v>394</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="10" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>232</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <v>496</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>155</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A20:H20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
pedoe solve 20 & 394
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Documents/Career @US/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="460" windowWidth="23860" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="1740" yWindow="460" windowWidth="23860" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -871,8 +871,8 @@
       <c r="D14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>28</v>
+      <c r="E14" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>35</v>
@@ -891,7 +891,7 @@
       <c r="D15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="10" t="s">
@@ -911,8 +911,8 @@
       <c r="D16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>28</v>
+      <c r="E16" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
add programing for linked list problem
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="43">
   <si>
     <t>#</t>
   </si>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,7 +609,9 @@
       <c r="E2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="G2" t="s">
         <v>29</v>
       </c>
@@ -653,7 +655,9 @@
       <c r="E4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="G4" t="s">
         <v>29</v>
       </c>
@@ -677,7 +681,9 @@
       <c r="E5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="G5" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
aton done 3 problems
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Documents/Career @US/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="460" windowWidth="23860" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="5880" yWindow="460" windowWidth="23860" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,14 +214,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFED7D31"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color rgb="FF4472C4"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -254,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -269,7 +261,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -556,7 +547,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,7 +600,7 @@
       <c r="E2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>35</v>
       </c>
       <c r="G2" t="s">
@@ -655,7 +646,7 @@
       <c r="E4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>35</v>
       </c>
       <c r="G4" t="s">
@@ -681,7 +672,7 @@
       <c r="E5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>35</v>
       </c>
       <c r="G5" t="s">
@@ -793,16 +784,16 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -880,7 +871,7 @@
       <c r="E14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -900,7 +891,7 @@
       <c r="E15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -920,7 +911,7 @@
       <c r="E16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -937,8 +928,8 @@
       <c r="D17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>28</v>
+      <c r="E17" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>18</v>
@@ -957,8 +948,8 @@
       <c r="D18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>28</v>
+      <c r="E18" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>18</v>
@@ -977,24 +968,24 @@
       <c r="D19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>28</v>
+      <c r="E19" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
pedoe choose 3 tree problems
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/Leetcode/Leetcode_github/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041B7381-982D-7148-BB4E-50DC0B8A1F24}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="460" windowWidth="37120" windowHeight="19720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
@@ -175,12 +174,21 @@
   </si>
   <si>
     <t>Tree</t>
+  </si>
+  <si>
+    <t>Find Largest Value in Each Tree Row</t>
+  </si>
+  <si>
+    <t>Sum of Left Leaves</t>
+  </si>
+  <si>
+    <t>Symmetric Tree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -559,11 +567,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,8 +964,8 @@
       <c r="D15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>27</v>
+      <c r="E15" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>47</v>
@@ -1153,6 +1161,75 @@
       </c>
       <c r="G23" s="5" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>515</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>404</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>101</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aton picked 3 tree questions
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Documents/Career @US/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="56">
   <si>
     <t>#</t>
   </si>
@@ -183,6 +183,18 @@
   </si>
   <si>
     <t>Symmetric Tree</t>
+  </si>
+  <si>
+    <t>Unique Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Convert Sorted Array to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Trim a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>April 4, 2018</t>
   </si>
 </sst>
 </file>
@@ -568,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1232,10 +1244,93 @@
         <v>34</v>
       </c>
     </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>96</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>108</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>669</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A30:I30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
INo picks tree assignments
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/LeetCodeMeeting/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A998316-7E89-B948-AF72-CFA0B9DFFAF7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="58">
   <si>
     <t>#</t>
   </si>
@@ -192,12 +193,21 @@
   </si>
   <si>
     <t>April 4, 2018</t>
+  </si>
+  <si>
+    <t>Same Tree</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>Add One Row to Tree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -576,11 +586,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1323,6 +1333,66 @@
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
     </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>100</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>226</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>623</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A10:I10"/>

</xml_diff>

<commit_message>
Aton picked 3 tree problems
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/LeetCodeMeeting/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Documents/Career @US/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A998316-7E89-B948-AF72-CFA0B9DFFAF7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="61">
   <si>
     <t>#</t>
   </si>
@@ -202,12 +201,21 @@
   </si>
   <si>
     <t>Add One Row to Tree</t>
+  </si>
+  <si>
+    <t>Binary Search Tree Iterator</t>
+  </si>
+  <si>
+    <t>Minimum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Binary Tree Path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -586,11 +594,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1393,6 +1401,66 @@
         <v>17</v>
       </c>
     </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>173</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>111</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>257</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A10:I10"/>

</xml_diff>

<commit_message>
pedoe pick 3 problems
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Documents/Career @US/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="64">
   <si>
     <t>#</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>Binary Tree Path</t>
+  </si>
+  <si>
+    <t>Find Bottom Left Tree Value</t>
+  </si>
+  <si>
+    <t>Second Minimum Node in a Binary Tree</t>
+  </si>
+  <si>
+    <t>Minimum Absolute Difference in BST</t>
   </si>
 </sst>
 </file>
@@ -595,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1461,6 +1470,66 @@
         <v>17</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
+        <v>513</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
+        <v>671</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>530</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A10:I10"/>

</xml_diff>

<commit_message>
Update solutions and status
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/FrontEnd/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/LeetCodeMeeting/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C8EAFF-1379-734C-9E6D-41ADA844A075}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="64">
   <si>
     <t>#</t>
   </si>
@@ -224,7 +225,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -603,11 +604,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1363,6 +1364,9 @@
       <c r="D31" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="E31" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F31" s="6" t="s">
         <v>45</v>
       </c>
@@ -1383,6 +1387,9 @@
       <c r="D32" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="E32" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F32" s="6" t="s">
         <v>45</v>
       </c>
@@ -1402,6 +1409,9 @@
       </c>
       <c r="D33" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
I-No picks 3 problems
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Documents/Career @US/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/LeetCodeMeeting/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632D50CA-3C86-4D4A-947D-D581F01959DB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36540" yWindow="3480" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="3480" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="68">
   <si>
     <t>#</t>
   </si>
@@ -219,12 +220,24 @@
   </si>
   <si>
     <t>Minimum Absolute Difference in BST</t>
+  </si>
+  <si>
+    <t>Find Mode in Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>Validate Binary Search Tree</t>
+  </si>
+  <si>
+    <t>April 17, 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -307,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,6 +335,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -603,11 +619,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1396,7 +1412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>623</v>
       </c>
@@ -1419,7 +1435,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>173</v>
       </c>
@@ -1442,7 +1458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>111</v>
       </c>
@@ -1465,7 +1481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>257</v>
       </c>
@@ -1488,7 +1504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>513</v>
       </c>
@@ -1511,7 +1527,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>671</v>
       </c>
@@ -1534,7 +1550,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>530</v>
       </c>
@@ -1557,11 +1573,88 @@
         <v>33</v>
       </c>
     </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
+        <v>501</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
+        <v>110</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="7">
+        <v>98</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A20:I20"/>
     <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A40:I40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Aton picked 3 questions
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/LeetCodeMeeting/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Google Drive/Career_USA/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632D50CA-3C86-4D4A-947D-D581F01959DB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="3480" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3540" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="71">
   <si>
     <t>#</t>
   </si>
@@ -232,12 +231,21 @@
   </si>
   <si>
     <t>April 17, 2018</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal II</t>
+  </si>
+  <si>
+    <t>Maximum Binary Tree</t>
+  </si>
+  <si>
+    <t>Two Sum IV - Input is a BST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -619,11 +627,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1649,6 +1657,66 @@
         <v>17</v>
       </c>
     </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
+        <v>107</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
+        <v>654</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
+        <v>653</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A10:I10"/>

</xml_diff>

<commit_message>
I-No picks DP problems
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Google Drive/Career_USA/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/LeetCodeMeeting/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EF1624-2F7D-D240-84A7-061C585562CD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36280" yWindow="2500" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="15060" yWindow="9620" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="79">
   <si>
     <t>#</t>
   </si>
@@ -249,12 +250,27 @@
   </si>
   <si>
     <t>Longest Univalue Path</t>
+  </si>
+  <si>
+    <t>April 30, 2018</t>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+  </si>
+  <si>
+    <t>Dynamic Programming</t>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+  </si>
+  <si>
+    <t>Counting Bits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -636,11 +652,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1670,7 +1686,9 @@
       <c r="D41" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E41" s="6"/>
+      <c r="E41" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F41" s="6" t="s">
         <v>45</v>
       </c>
@@ -1691,7 +1709,9 @@
       <c r="D42" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="6"/>
+      <c r="E42" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F42" s="6" t="s">
         <v>45</v>
       </c>
@@ -1712,7 +1732,9 @@
       <c r="D43" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F43" s="3" t="s">
         <v>46</v>
       </c>
@@ -1829,7 +1851,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>687</v>
       </c>
@@ -1849,12 +1871,86 @@
         <v>33</v>
       </c>
     </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
+        <v>53</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="7">
+        <v>70</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
+        <v>338</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A20:I20"/>
     <mergeCell ref="A30:I30"/>
     <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A50:I50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Upload answers and update status
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Google Drive/Career_USA/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/LeetCodeMeeting/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D34E77-CFFA-C645-B5CD-869BA7E61E0E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42660" yWindow="7580" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="22800" yWindow="8300" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="85">
   <si>
     <t>#</t>
   </si>
@@ -287,7 +288,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -669,11 +670,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1923,6 +1924,9 @@
       <c r="D51" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="E51" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F51" s="6" t="s">
         <v>45</v>
       </c>
@@ -1943,6 +1947,9 @@
       <c r="D52" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="E52" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F52" s="6" t="s">
         <v>45</v>
       </c>
@@ -1962,6 +1969,9 @@
       </c>
       <c r="D53" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Aton picked 3 questions: q exit
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/Interview/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilan/Google Drive/Career_USA/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13700" tabRatio="500"/>
+    <workbookView xWindow="37700" yWindow="460" windowWidth="29340" windowHeight="18180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="89">
   <si>
     <t>#</t>
   </si>
@@ -282,6 +282,18 @@
   </si>
   <si>
     <t>Range Sum Query - Immutable</t>
+  </si>
+  <si>
+    <t>May 6, 2018</t>
+  </si>
+  <si>
+    <t>Perfect Square</t>
+  </si>
+  <si>
+    <t>Unique Paths</t>
+  </si>
+  <si>
+    <t>Triangle</t>
   </si>
 </sst>
 </file>
@@ -370,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -390,6 +402,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1712,6 +1725,9 @@
       <c r="G41" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H41" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
@@ -1735,6 +1751,9 @@
       <c r="G42" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H42" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
@@ -1758,6 +1777,9 @@
       <c r="G43" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H43" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
@@ -1781,6 +1803,9 @@
       <c r="G44" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H44" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
@@ -1804,6 +1829,9 @@
       <c r="G45" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H45" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
@@ -1827,6 +1855,9 @@
       <c r="G46" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H46" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
@@ -1850,6 +1881,9 @@
       <c r="G47" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="H47" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
@@ -1873,6 +1907,9 @@
       <c r="G48" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="H48" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
@@ -1895,6 +1932,9 @@
       </c>
       <c r="G49" s="5" t="s">
         <v>33</v>
+      </c>
+      <c r="H49" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -1932,6 +1972,9 @@
       <c r="G51" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H51" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
@@ -1955,6 +1998,9 @@
       <c r="G52" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H52" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
@@ -1978,6 +2024,9 @@
       <c r="G53" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H53" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
@@ -2001,6 +2050,9 @@
       <c r="G54" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="H54" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
@@ -2024,6 +2076,9 @@
       <c r="G55" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="H55" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
@@ -2047,6 +2102,9 @@
       <c r="G56" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="H56" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
@@ -2070,6 +2128,9 @@
       <c r="G57" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H57" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
@@ -2093,6 +2154,9 @@
       <c r="G58" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H58" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
@@ -2116,9 +2180,89 @@
       <c r="G59" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="11">
+        <v>279</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="6"/>
+      <c r="F61" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="11">
+        <v>62</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62" t="s">
+        <v>76</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="6"/>
+      <c r="F62" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="11">
+        <v>120</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="6"/>
+      <c r="F63" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A60:I60"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A20:I20"/>
     <mergeCell ref="A30:I30"/>

</xml_diff>

<commit_message>
Update progress and solutions
</commit_message>
<xml_diff>
--- a/Leetcode Progress.xlsx
+++ b/Leetcode Progress.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedoe/Documents/Interview/Dream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/INo/Google Drive/Programming/LeetCodeMeeting/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BC5579-7ABE-A74F-A0D4-1DA670EEC22C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="1300" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="95">
   <si>
     <t>#</t>
   </si>
@@ -317,7 +318,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -700,11 +701,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2297,6 +2298,9 @@
       <c r="D64" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="E64" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F64" s="3" t="s">
         <v>46</v>
       </c>
@@ -2317,6 +2321,9 @@
       <c r="D65" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="E65" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F65" s="3" t="s">
         <v>46</v>
       </c>
@@ -2336,6 +2343,9 @@
       </c>
       <c r="D66" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>46</v>

</xml_diff>